<commit_message>
Added test workflows for arena, removed old stuff
</commit_message>
<xml_diff>
--- a/backend/arena/evaluation.xlsx
+++ b/backend/arena/evaluation.xlsx
@@ -14,9 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
   <si>
     <t>create</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
   </si>
   <si>
     <t>False</t>
@@ -421,16 +424,18 @@
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
       <c r="D1" s="3"/>
       <c r="E1" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="4">
@@ -440,10 +445,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
       <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="4">
@@ -453,10 +458,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
       <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="4">
@@ -466,10 +471,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="4">

</xml_diff>